<commit_message>
updated with statistics script in R
</commit_message>
<xml_diff>
--- a/Lectures/Problem_Set_1.xlsx
+++ b/Lectures/Problem_Set_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14800" yWindow="0" windowWidth="15980" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="6760" yWindow="0" windowWidth="21000" windowHeight="16940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Variance</t>
   </si>
@@ -42,9 +42,6 @@
     <t>mean</t>
   </si>
   <si>
-    <t>variance</t>
-  </si>
-  <si>
     <t>sd</t>
   </si>
   <si>
@@ -55,6 +52,15 @@
   </si>
   <si>
     <t>- 95% confidence interval</t>
+  </si>
+  <si>
+    <t>variance (of sample so s^2 = sum of all (data-mean)^2 / n-1</t>
+  </si>
+  <si>
+    <t>CV = sd/mean * 100</t>
+  </si>
+  <si>
+    <t>se = sd / sqrt(n)</t>
   </si>
 </sst>
 </file>
@@ -111,8 +117,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -127,15 +143,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,6 +217,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
@@ -198,30 +232,30 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$17:$H$17</c:f>
+                <c:f>Sheet1!$H$17:$I$17</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.635609943282828</c:v>
+                    <c:v>1.238726945070803</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.175159563633807</c:v>
+                    <c:v>0.669991708074726</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$17:$H$17</c:f>
+                <c:f>Sheet1!$H$17:$I$17</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.635609943282828</c:v>
+                    <c:v>1.238726945070803</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.175159563633807</c:v>
+                    <c:v>0.669991708074726</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -229,29 +263,29 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$14:$H$14</c:f>
+              <c:f>Sheet1!$H$14:$I$14</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Top</c:v>
+                  <c:v>Bottom</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bottom</c:v>
+                  <c:v>Top</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$15:$H$15</c:f>
+              <c:f>Sheet1!$H$15:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3.6</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -265,12 +299,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2123044088"/>
-        <c:axId val="2123331048"/>
+        <c:gapWidth val="15"/>
+        <c:axId val="2056476296"/>
+        <c:axId val="2098610248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123044088"/>
+        <c:axId val="2056476296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,7 +337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123331048"/>
+        <c:crossAx val="2098610248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -311,13 +345,21 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123331048"/>
+        <c:axId val="2098610248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -346,9 +388,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123044088"/>
+        <c:crossAx val="2056476296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2.5"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -367,16 +410,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -722,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -738,12 +781,22 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2">
+        <f>AVERAGE(A2:A11)</f>
         <v>5.3</v>
       </c>
       <c r="C2">
@@ -751,8 +804,20 @@
         <v>0.49000000000000027</v>
       </c>
       <c r="D2">
-        <f>C12/10</f>
-        <v>6.2100000000000017</v>
+        <f>C12/9</f>
+        <v>6.9000000000000021</v>
+      </c>
+      <c r="E2">
+        <f>SQRT(D2)</f>
+        <v>2.62678510731274</v>
+      </c>
+      <c r="F2">
+        <f>E2/SQRT(10)</f>
+        <v>0.83066238629180755</v>
+      </c>
+      <c r="G2">
+        <f>E2/B2*100</f>
+        <v>49.56198315684415</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -862,11 +927,11 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
       <c r="H14" t="s">
         <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -884,14 +949,14 @@
         <f>(B15-$B$25)^2</f>
         <v>18.489999999999998</v>
       </c>
-      <c r="G15">
-        <v>3.6</v>
+      <c r="G15" t="s">
+        <v>6</v>
       </c>
       <c r="H15">
         <v>7.3</v>
       </c>
-      <c r="I15" t="s">
-        <v>6</v>
+      <c r="I15">
+        <v>3.6</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -902,21 +967,23 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:E24" si="1">(A16-$A$25)^2</f>
+        <f t="shared" ref="D16:D24" si="1">(A16-$A$25)^2</f>
         <v>6.7600000000000007</v>
       </c>
       <c r="E16">
         <f t="shared" ref="E16:E24" si="2">(B16-$B$25)^2</f>
         <v>22.090000000000003</v>
       </c>
-      <c r="G16">
-        <v>2.0099751242241779</v>
+      <c r="G16" t="s">
+        <v>7</v>
       </c>
       <c r="H16">
-        <v>3.7161808352124091</v>
-      </c>
-      <c r="I16" t="s">
-        <v>8</v>
+        <f>B27</f>
+        <v>3.9171985454460239</v>
+      </c>
+      <c r="I16">
+        <f>A27</f>
+        <v>2.1186998109427608</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -934,16 +1001,16 @@
         <f t="shared" si="2"/>
         <v>18.489999999999998</v>
       </c>
-      <c r="G17">
-        <f>G16/SQRT(10)</f>
-        <v>0.63560994328282805</v>
+      <c r="G17" t="s">
+        <v>8</v>
       </c>
       <c r="H17">
         <f>H16/SQRT(10)</f>
-        <v>1.175159563633807</v>
-      </c>
-      <c r="I17" t="s">
-        <v>9</v>
+        <v>1.2387269450708029</v>
+      </c>
+      <c r="I17">
+        <f>I16/SQRT(10)</f>
+        <v>0.66999170807472608</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1060,11 +1127,11 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <f>SUM(A15:A24)/10</f>
+        <f>AVERAGE(A15:A24)</f>
         <v>3.6</v>
       </c>
       <c r="B25">
-        <f>SUM(B15:B24)/10</f>
+        <f>AVERAGE(B15:B24)</f>
         <v>7.3</v>
       </c>
       <c r="C25" t="s">
@@ -1081,54 +1148,54 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <f>D25/10</f>
-        <v>4.04</v>
+        <f>D25/9</f>
+        <v>4.4888888888888889</v>
       </c>
       <c r="B26">
-        <f>E25/10</f>
-        <v>13.809999999999997</v>
+        <f>E25/9</f>
+        <v>15.344444444444441</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <f>SQRT(A26)</f>
-        <v>2.0099751242241779</v>
+        <f>STDEV(A15:A24)</f>
+        <v>2.1186998109427608</v>
       </c>
       <c r="B27">
-        <f>SQRT(B26)</f>
-        <v>3.7161808352124091</v>
+        <f>STDEV(B15:B24)</f>
+        <v>3.9171985454460239</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
         <f>A25+A27*1.96</f>
-        <v>7.539551243479389</v>
+        <v>7.7526516294478114</v>
       </c>
       <c r="B28">
         <f>B25+B27*1.96</f>
-        <v>14.583714437016322</v>
+        <v>14.977709149074206</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
         <f>A25-A27*1.96</f>
-        <v>-0.33955124347938836</v>
+        <v>-0.55265162944781077</v>
       </c>
       <c r="B29">
         <f>B25-B27*1.96</f>
-        <v>1.6285562983678226E-2</v>
+        <v>-0.37770914907420661</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>